<commit_message>
create local directories structure to store data
</commit_message>
<xml_diff>
--- a/test/data/task_summary.xlsx
+++ b/test/data/task_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,37 +483,286 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sbkzbz</t>
+          <t>sbkuzh</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>task_2024-07-07_ZBZ_SMALL_READY</t>
+          <t>task_2050-01-01_UZH_LARGE_READY</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-07-05 06:57:18</t>
+          <t>2024-07-15 18:01:55</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-07-07</t>
+          <t>2050-01-01</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>LARGE</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>READY</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sbkrzs</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>task_2034-01-01_RZS_LARGE_ERROR</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2034-01-01</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>LARGE</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Missing file task_2034-01-01_RZS_LARGE.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sbkrzs</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>task_2033-01-01_RZS_LARGE_ERROR</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2033-01-01</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>LARGE</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Missing file task_2033-01-01_RZS_LARGE.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>sbkzbs</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>task_2033-01-01_ZBS_LARGE_ERROR</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2033-01-01</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>LARGE</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>A large task is already scheduled for this date</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>sbkrzs</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>task_2041-01-01_UBS_LARGE_ERROR</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2041-01-01</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>LARGE</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Missing file task_2041-01-01_UBS_LARGE.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>sbkrzs</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>task_2032-01-01_RZS_LARGE_ERROR</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2032-01-01</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>LARGE</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Missing file task_2032-01-01_RZS_LARGE.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>sbkzbz</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>task_2024-07-17_ZBZ_SMALL_READY</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2024-07-15 18:02:42</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2024-07-17</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>SMALL</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>READY</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>sbkhsg</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>task_2024-07-15_HSG_SMALL_DONE</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2024-07-15 18:02:50</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2024-07-15 18:03:00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2024-07-15</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>SMALL</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add storage_tasks in upload directory
</commit_message>
<xml_diff>
--- a/test/data/task_summary.xlsx
+++ b/test/data/task_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,29 +483,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sbkuzh</t>
+          <t>sbkzbz</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>task_2050-01-01_UZH_LARGE_READY</t>
+          <t>task_2024-07-21_ZBZ_SMALL_READY</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-07-18 21:15:38</t>
+          <t>2024-07-19 12:27:41</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2050-01-01</t>
+          <t>2024-07-21</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>LARGE</t>
+          <t>SMALL</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -514,255 +514,6 @@
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>sbkrzs</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>task_2034-01-01_RZS_LARGE_ERROR</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2034-01-01</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>LARGE</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>ERROR</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Missing file task_2034-01-01_RZS_LARGE.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>sbkrzs</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>task_2033-01-01_RZS_LARGE_ERROR</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2033-01-01</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>LARGE</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>ERROR</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Missing file task_2033-01-01_RZS_LARGE.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>sbkzbs</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>task_2033-01-01_ZBS_LARGE_ERROR</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2033-01-01</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>LARGE</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>ERROR</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>A large task is already scheduled for this date</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>sbkrzs</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>task_2041-01-01_UBS_LARGE_ERROR</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2041-01-01</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>LARGE</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>ERROR</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Missing file task_2041-01-01_UBS_LARGE.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>sbkrzs</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>task_2032-01-01_RZS_LARGE_ERROR</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2032-01-01</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>LARGE</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>ERROR</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Missing file task_2032-01-01_RZS_LARGE.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>sbkzbz</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>task_2024-07-20_ZBZ_SMALL_READY</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2024-07-18 21:16:33</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2024-07-20</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>SMALL</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>READY</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>sbkhsg</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>task_2024-07-18_HSG_SMALL_DONE</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2024-07-18 21:16:43</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2024-07-18 21:16:53</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2024-07-18</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>SMALL</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>DONE</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
allow rewrite task with error
</commit_message>
<xml_diff>
--- a/test/data/task_summary.xlsx
+++ b/test/data/task_summary.xlsx
@@ -493,7 +493,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-07-20 00:40:59</t>
+          <t>2024-07-24 11:41:01</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -698,19 +698,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>task_2024-07-22_ZBZ_SMALL_READY</t>
+          <t>task_2024-07-26_ZBZ_SMALL_READY</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024-07-20 00:41:56</t>
+          <t>2024-07-24 11:41:55</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2024-07-22</t>
+          <t>2024-07-26</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -733,23 +733,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>task_2024-07-20_HSG_SMALL_DONE</t>
+          <t>task_2024-07-24_HSG_SMALL_DONE</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2024-07-20 00:42:06</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
+          <t>2024-07-24 11:42:05</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2024-07-24 11:42:08</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2024-07-20 00:42:16</t>
+          <t>2024-07-24 11:42:15</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2024-07-20</t>
+          <t>2024-07-24</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">

</xml_diff>

<commit_message>
fix error when task summary is missing
</commit_message>
<xml_diff>
--- a/test/data/task_summary.xlsx
+++ b/test/data/task_summary.xlsx
@@ -493,7 +493,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-07-24 12:03:31</t>
+          <t>2024-07-24 13:54:44</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -703,7 +703,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024-07-24 12:04:25</t>
+          <t>2024-07-24 13:55:40</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -738,7 +738,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2024-07-24 12:04:49</t>
+          <t>2024-07-24 13:56:03</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -773,17 +773,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2024-07-24 12:04:59</t>
+          <t>2024-07-24 13:56:13</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-07-24 12:05:02</t>
+          <t>2024-07-24 13:56:16</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2024-07-24 12:05:08</t>
+          <t>2024-07-24 13:56:22</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">

</xml_diff>

<commit_message>
delete task before creating new ones
</commit_message>
<xml_diff>
--- a/test/data/task_summary.xlsx
+++ b/test/data/task_summary.xlsx
@@ -493,7 +493,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-07-24 13:54:44</t>
+          <t>2024-08-23 17:23:09</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -698,19 +698,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>task_2024-07-26_ZBZ_SMALL_READY</t>
+          <t>task_2024-08-25_ZBZ_SMALL_READY</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024-07-24 13:55:40</t>
+          <t>2024-08-23 17:25:57</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2024-07-26</t>
+          <t>2024-08-25</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -733,19 +733,19 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>task_2024-07-29_ZBZ3_SMALL_READY</t>
+          <t>task_2024-08-28_ZBZ3_SMALL_READY</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2024-07-24 13:56:03</t>
+          <t>2024-08-23 17:27:03</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2024-07-29</t>
+          <t>2024-08-28</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -768,27 +768,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>task_2024-07-24_HSG_SMALL_DONE</t>
+          <t>task_2024-08-23_HSG_SMALL_DONE</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2024-07-24 13:56:13</t>
+          <t>2024-08-23 17:27:32</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-07-24 13:56:16</t>
+          <t>2024-08-23 17:27:40</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2024-07-24 13:56:22</t>
+          <t>2024-08-23 17:27:52</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2024-07-24</t>
+          <t>2024-08-23</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">

</xml_diff>